<commit_message>
add data and read-in code
</commit_message>
<xml_diff>
--- a/stimuli/NAD_field.xlsx
+++ b/stimuli/NAD_field.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terminalpc\Documents\GitHub\Yeli-NAD\stimuli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcas\Documents\GitHub\Yeli-NAD\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384265DA-76DC-4267-9D81-4C42540A9CDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,10 @@
     <sheet name="word_files_appfriendly" sheetId="5" r:id="rId4"/>
     <sheet name="lexicons" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">word_files_appfriendly!$A$1:$L$82</definedName>
+  </definedNames>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2210" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2210" uniqueCount="257">
   <si>
     <t>p</t>
   </si>
@@ -813,11 +815,38 @@
   <si>
     <t>exp2</t>
   </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2160,7 +2189,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4150,7 +4179,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S132"/>
   <sheetViews>
     <sheetView topLeftCell="A88" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -5875,7 +5904,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -7805,17 +7834,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="13" customWidth="1"/>
     <col min="12" max="12" width="16.1796875" bestFit="1" customWidth="1"/>
@@ -8902,7 +8931,7 @@
         <v>141</v>
       </c>
       <c r="F29" s="62" t="s">
-        <v>136</v>
+        <v>252</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>203</v>
@@ -8940,7 +8969,7 @@
         <v>142</v>
       </c>
       <c r="F30" s="62" t="s">
-        <v>139</v>
+        <v>255</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>203</v>
@@ -8978,7 +9007,7 @@
         <v>143</v>
       </c>
       <c r="F31" s="62" t="s">
-        <v>135</v>
+        <v>251</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>203</v>
@@ -9016,7 +9045,7 @@
         <v>144</v>
       </c>
       <c r="F32" s="62" t="s">
-        <v>91</v>
+        <v>249</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>203</v>
@@ -9054,7 +9083,7 @@
         <v>145</v>
       </c>
       <c r="F33" s="62" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>203</v>
@@ -9092,7 +9121,7 @@
         <v>146</v>
       </c>
       <c r="F34" s="62" t="s">
-        <v>140</v>
+        <v>256</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>203</v>
@@ -9130,7 +9159,7 @@
         <v>147</v>
       </c>
       <c r="F35" s="62" t="s">
-        <v>138</v>
+        <v>254</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>203</v>
@@ -9168,7 +9197,7 @@
         <v>148</v>
       </c>
       <c r="F36" s="62" t="s">
-        <v>90</v>
+        <v>248</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>203</v>
@@ -9206,7 +9235,7 @@
         <v>149</v>
       </c>
       <c r="F37" s="62" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>203</v>
@@ -9244,7 +9273,7 @@
         <v>153</v>
       </c>
       <c r="F38" s="62" t="s">
-        <v>90</v>
+        <v>248</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>76</v>
@@ -9282,7 +9311,7 @@
         <v>154</v>
       </c>
       <c r="F39" s="62" t="s">
-        <v>91</v>
+        <v>249</v>
       </c>
       <c r="G39" s="62" t="s">
         <v>77</v>
@@ -9320,7 +9349,7 @@
         <v>155</v>
       </c>
       <c r="F40" s="62" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="G40" s="62" t="s">
         <v>77</v>
@@ -9358,7 +9387,7 @@
         <v>156</v>
       </c>
       <c r="F41" s="62" t="s">
-        <v>135</v>
+        <v>251</v>
       </c>
       <c r="G41" s="62" t="s">
         <v>78</v>
@@ -9396,7 +9425,7 @@
         <v>157</v>
       </c>
       <c r="F42" s="62" t="s">
-        <v>136</v>
+        <v>252</v>
       </c>
       <c r="G42" s="62" t="s">
         <v>76</v>
@@ -9434,7 +9463,7 @@
         <v>158</v>
       </c>
       <c r="F43" s="62" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="G43" s="62" t="s">
         <v>78</v>
@@ -9472,7 +9501,7 @@
         <v>159</v>
       </c>
       <c r="F44" s="62" t="s">
-        <v>138</v>
+        <v>254</v>
       </c>
       <c r="G44" s="62" t="s">
         <v>78</v>
@@ -9510,7 +9539,7 @@
         <v>160</v>
       </c>
       <c r="F45" s="62" t="s">
-        <v>139</v>
+        <v>255</v>
       </c>
       <c r="G45" s="62" t="s">
         <v>77</v>
@@ -9548,7 +9577,7 @@
         <v>161</v>
       </c>
       <c r="F46" s="62" t="s">
-        <v>140</v>
+        <v>256</v>
       </c>
       <c r="G46" s="62" t="s">
         <v>76</v>
@@ -10270,7 +10299,7 @@
         <v>141</v>
       </c>
       <c r="F65" s="62" t="s">
-        <v>90</v>
+        <v>248</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>203</v>
@@ -10308,7 +10337,7 @@
         <v>142</v>
       </c>
       <c r="F66" s="62" t="s">
-        <v>91</v>
+        <v>249</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>203</v>
@@ -10346,7 +10375,7 @@
         <v>143</v>
       </c>
       <c r="F67" s="62" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>203</v>
@@ -10384,7 +10413,7 @@
         <v>144</v>
       </c>
       <c r="F68" s="62" t="s">
-        <v>135</v>
+        <v>251</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>203</v>
@@ -10422,7 +10451,7 @@
         <v>145</v>
       </c>
       <c r="F69" s="62" t="s">
-        <v>136</v>
+        <v>252</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>203</v>
@@ -10460,7 +10489,7 @@
         <v>146</v>
       </c>
       <c r="F70" s="62" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>203</v>
@@ -10498,7 +10527,7 @@
         <v>147</v>
       </c>
       <c r="F71" s="62" t="s">
-        <v>138</v>
+        <v>254</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>203</v>
@@ -10536,7 +10565,7 @@
         <v>148</v>
       </c>
       <c r="F72" s="62" t="s">
-        <v>139</v>
+        <v>255</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>203</v>
@@ -10574,7 +10603,7 @@
         <v>149</v>
       </c>
       <c r="F73" s="62" t="s">
-        <v>140</v>
+        <v>256</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>203</v>
@@ -10612,7 +10641,7 @@
         <v>225</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>90</v>
+        <v>248</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>203</v>
@@ -10650,7 +10679,7 @@
         <v>228</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>135</v>
+        <v>251</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>203</v>
@@ -10688,7 +10717,7 @@
         <v>227</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>91</v>
+        <v>249</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>203</v>
@@ -10726,7 +10755,7 @@
         <v>229</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>203</v>
@@ -10764,7 +10793,7 @@
         <v>226</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>139</v>
+        <v>255</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>203</v>
@@ -10802,7 +10831,7 @@
         <v>230</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>203</v>
@@ -10840,7 +10869,7 @@
         <v>231</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>140</v>
+        <v>256</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>203</v>
@@ -10878,7 +10907,7 @@
         <v>232</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>138</v>
+        <v>254</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>203</v>
@@ -10916,7 +10945,7 @@
         <v>233</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>136</v>
+        <v>252</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>203</v>
@@ -10938,6 +10967,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:L82">
+    <sortCondition ref="A1"/>
+  </sortState>
   <conditionalFormatting sqref="E38:E46">
     <cfRule type="duplicateValues" dxfId="25" priority="46"/>
   </conditionalFormatting>
@@ -11022,11 +11054,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>